<commit_message>
++ update template customer contract
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CustomerContractImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CustomerContractImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\eFms\WebAPI\eFMS.API.SystemWeb\eFMS.API.Catalogue\eFMS.API.Catalogue\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -195,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -280,7 +280,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -576,7 +576,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update file exe import contract
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CustomerContractImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CustomerContractImportTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="15900" windowHeight="8235"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="15900" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Contract" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Payment Term/Trial Day</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>HĐ00902</t>
-  </si>
-  <si>
-    <t>Guaranteed</t>
   </si>
 </sst>
 </file>
@@ -841,7 +838,7 @@
         <v>42</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>13</v>

</xml_diff>